<commit_message>
Made code shorter, py3.6+
Added f-strings
Created class to process optimization outputs
</commit_message>
<xml_diff>
--- a/further_parameters.xlsx
+++ b/further_parameters.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GIT\journal_papers\besopt_rebuttal\Energy_2016_a\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GIT\GitHub\BESopt\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBA57BA7-C2EA-4ADF-B88D-17BD33EA58CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14385" yWindow="-15" windowWidth="14430" windowHeight="12855" activeTab="3"/>
+    <workbookView xWindow="-28920" yWindow="-1065" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="gen_economics" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,17 @@
     <sheet name="co2_emissions" sheetId="3" r:id="rId5"/>
     <sheet name="tariff_example" sheetId="5" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -634,7 +645,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -695,8 +706,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Link" xfId="1" builtinId="8"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -712,7 +723,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -787,6 +798,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -822,6 +850,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -997,14 +1042,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="40.7109375" customWidth="1"/>
@@ -1425,17 +1470,17 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D13" r:id="rId1"/>
-    <hyperlink ref="D17" r:id="rId2"/>
-    <hyperlink ref="D18" r:id="rId3"/>
-    <hyperlink ref="D14" r:id="rId4"/>
-    <hyperlink ref="D16" r:id="rId5"/>
-    <hyperlink ref="D15" r:id="rId6"/>
-    <hyperlink ref="D7" r:id="rId7"/>
-    <hyperlink ref="D8" r:id="rId8"/>
-    <hyperlink ref="D10" r:id="rId9"/>
-    <hyperlink ref="D9" r:id="rId10"/>
-    <hyperlink ref="D19" r:id="rId11"/>
+    <hyperlink ref="D13" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="D17" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="D18" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="D14" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="D16" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="D15" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="D7" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="D8" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="D10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="D9" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="D19" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId12"/>
@@ -1443,14 +1488,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="51.85546875" customWidth="1"/>
@@ -1571,22 +1616,22 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E6" r:id="rId1"/>
-    <hyperlink ref="E7" r:id="rId2"/>
+    <hyperlink ref="E6" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="E7" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="61.140625" customWidth="1"/>
     <col min="3" max="3" width="65" customWidth="1"/>
@@ -1717,21 +1762,21 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F6" r:id="rId1"/>
+    <hyperlink ref="F6" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
@@ -1797,8 +1842,8 @@
         <v>36</v>
       </c>
       <c r="B5">
-        <f>3600*5</f>
-        <v>18000</v>
+        <f>3600*0.5</f>
+        <v>1800</v>
       </c>
       <c r="C5" t="s">
         <v>28</v>
@@ -1911,26 +1956,26 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:O104"/>
   <sheetViews>
     <sheetView topLeftCell="E74" workbookViewId="0">
       <selection activeCell="N99" sqref="N99:O99"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="33.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
@@ -2016,7 +2061,7 @@
       </c>
       <c r="O3" t="str">
         <f t="shared" ref="O3:O17" si="0">CONCATENATE(O2,I3, " - ",J3,": ",L3,"; ")</f>
-        <v xml:space="preserve">[0 - 5: 0.0463; </v>
+        <v xml:space="preserve">[0 - 5: 0,0463; </v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -2037,11 +2082,11 @@
       </c>
       <c r="N4" t="str">
         <f t="shared" ref="N4:N17" si="1">CONCATENATE(N3,I4, " - ",J4,": ",K4,"; ")</f>
-        <v xml:space="preserve">[0 - 5: 120; 5 - 10: 79.08; </v>
+        <v xml:space="preserve">[0 - 5: 120; 5 - 10: 79,08; </v>
       </c>
       <c r="O4" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">[0 - 5: 0.0463; 5 - 10: 0.0448; </v>
+        <v xml:space="preserve">[0 - 5: 0,0463; 5 - 10: 0,0448; </v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -2071,11 +2116,11 @@
       </c>
       <c r="N5" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">[0 - 5: 120; 5 - 10: 79.08; 10 - 15: 89.76; </v>
+        <v xml:space="preserve">[0 - 5: 120; 5 - 10: 79,08; 10 - 15: 89,76; </v>
       </c>
       <c r="O5" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">[0 - 5: 0.0463; 5 - 10: 0.0448; 10 - 15: 0.0417; </v>
+        <v xml:space="preserve">[0 - 5: 0,0463; 5 - 10: 0,0448; 10 - 15: 0,0417; </v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -2111,11 +2156,11 @@
       </c>
       <c r="N6" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">[0 - 5: 120; 5 - 10: 79.08; 10 - 15: 89.76; 15 - 20: 86.28; </v>
+        <v xml:space="preserve">[0 - 5: 120; 5 - 10: 79,08; 10 - 15: 89,76; 15 - 20: 86,28; </v>
       </c>
       <c r="O6" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">[0 - 5: 0.0463; 5 - 10: 0.0448; 10 - 15: 0.0417; 15 - 20: 0.0401; </v>
+        <v xml:space="preserve">[0 - 5: 0,0463; 5 - 10: 0,0448; 10 - 15: 0,0417; 15 - 20: 0,0401; </v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
@@ -2151,11 +2196,11 @@
       </c>
       <c r="N7" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">[0 - 5: 120; 5 - 10: 79.08; 10 - 15: 89.76; 15 - 20: 86.28; 20 - 25: 0; </v>
+        <v xml:space="preserve">[0 - 5: 120; 5 - 10: 79,08; 10 - 15: 89,76; 15 - 20: 86,28; 20 - 25: 0; </v>
       </c>
       <c r="O7" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">[0 - 5: 0.0463; 5 - 10: 0.0448; 10 - 15: 0.0417; 15 - 20: 0.0401; 20 - 25: 0.0439; </v>
+        <v xml:space="preserve">[0 - 5: 0,0463; 5 - 10: 0,0448; 10 - 15: 0,0417; 15 - 20: 0,0401; 20 - 25: 0,0439; </v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
@@ -2173,11 +2218,11 @@
       </c>
       <c r="N8" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">[0 - 5: 120; 5 - 10: 79.08; 10 - 15: 89.76; 15 - 20: 86.28; 20 - 25: 0; 25 - 30: 0; </v>
+        <v xml:space="preserve">[0 - 5: 120; 5 - 10: 79,08; 10 - 15: 89,76; 15 - 20: 86,28; 20 - 25: 0; 25 - 30: 0; </v>
       </c>
       <c r="O8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">[0 - 5: 0.0463; 5 - 10: 0.0448; 10 - 15: 0.0417; 15 - 20: 0.0401; 20 - 25: 0.0439; 25 - 30: 0.0434; </v>
+        <v xml:space="preserve">[0 - 5: 0,0463; 5 - 10: 0,0448; 10 - 15: 0,0417; 15 - 20: 0,0401; 20 - 25: 0,0439; 25 - 30: 0,0434; </v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
@@ -2195,11 +2240,11 @@
       </c>
       <c r="N9" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">[0 - 5: 120; 5 - 10: 79.08; 10 - 15: 89.76; 15 - 20: 86.28; 20 - 25: 0; 25 - 30: 0; 30 - 35: 0; </v>
+        <v xml:space="preserve">[0 - 5: 120; 5 - 10: 79,08; 10 - 15: 89,76; 15 - 20: 86,28; 20 - 25: 0; 25 - 30: 0; 30 - 35: 0; </v>
       </c>
       <c r="O9" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">[0 - 5: 0.0463; 5 - 10: 0.0448; 10 - 15: 0.0417; 15 - 20: 0.0401; 20 - 25: 0.0439; 25 - 30: 0.0434; 30 - 35: 0.0426; </v>
+        <v xml:space="preserve">[0 - 5: 0,0463; 5 - 10: 0,0448; 10 - 15: 0,0417; 15 - 20: 0,0401; 20 - 25: 0,0439; 25 - 30: 0,0434; 30 - 35: 0,0426; </v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
@@ -2217,11 +2262,11 @@
       </c>
       <c r="N10" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">[0 - 5: 120; 5 - 10: 79.08; 10 - 15: 89.76; 15 - 20: 86.28; 20 - 25: 0; 25 - 30: 0; 30 - 35: 0; 35 - 40: 0; </v>
+        <v xml:space="preserve">[0 - 5: 120; 5 - 10: 79,08; 10 - 15: 89,76; 15 - 20: 86,28; 20 - 25: 0; 25 - 30: 0; 30 - 35: 0; 35 - 40: 0; </v>
       </c>
       <c r="O10" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">[0 - 5: 0.0463; 5 - 10: 0.0448; 10 - 15: 0.0417; 15 - 20: 0.0401; 20 - 25: 0.0439; 25 - 30: 0.0434; 30 - 35: 0.0426; 35 - 40: 0.0422; </v>
+        <v xml:space="preserve">[0 - 5: 0,0463; 5 - 10: 0,0448; 10 - 15: 0,0417; 15 - 20: 0,0401; 20 - 25: 0,0439; 25 - 30: 0,0434; 30 - 35: 0,0426; 35 - 40: 0,0422; </v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
@@ -2239,11 +2284,11 @@
       </c>
       <c r="N11" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">[0 - 5: 120; 5 - 10: 79.08; 10 - 15: 89.76; 15 - 20: 86.28; 20 - 25: 0; 25 - 30: 0; 30 - 35: 0; 35 - 40: 0; 40 - 45: 0; </v>
+        <v xml:space="preserve">[0 - 5: 120; 5 - 10: 79,08; 10 - 15: 89,76; 15 - 20: 86,28; 20 - 25: 0; 25 - 30: 0; 30 - 35: 0; 35 - 40: 0; 40 - 45: 0; </v>
       </c>
       <c r="O11" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">[0 - 5: 0.0463; 5 - 10: 0.0448; 10 - 15: 0.0417; 15 - 20: 0.0401; 20 - 25: 0.0439; 25 - 30: 0.0434; 30 - 35: 0.0426; 35 - 40: 0.0422; 40 - 45: 0.0417; </v>
+        <v xml:space="preserve">[0 - 5: 0,0463; 5 - 10: 0,0448; 10 - 15: 0,0417; 15 - 20: 0,0401; 20 - 25: 0,0439; 25 - 30: 0,0434; 30 - 35: 0,0426; 35 - 40: 0,0422; 40 - 45: 0,0417; </v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
@@ -2261,11 +2306,11 @@
       </c>
       <c r="N12" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">[0 - 5: 120; 5 - 10: 79.08; 10 - 15: 89.76; 15 - 20: 86.28; 20 - 25: 0; 25 - 30: 0; 30 - 35: 0; 35 - 40: 0; 40 - 45: 0; 45 - 50: 0; </v>
+        <v xml:space="preserve">[0 - 5: 120; 5 - 10: 79,08; 10 - 15: 89,76; 15 - 20: 86,28; 20 - 25: 0; 25 - 30: 0; 30 - 35: 0; 35 - 40: 0; 40 - 45: 0; 45 - 50: 0; </v>
       </c>
       <c r="O12" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">[0 - 5: 0.0463; 5 - 10: 0.0448; 10 - 15: 0.0417; 15 - 20: 0.0401; 20 - 25: 0.0439; 25 - 30: 0.0434; 30 - 35: 0.0426; 35 - 40: 0.0422; 40 - 45: 0.0417; 45 - 50: 0.0414; </v>
+        <v xml:space="preserve">[0 - 5: 0,0463; 5 - 10: 0,0448; 10 - 15: 0,0417; 15 - 20: 0,0401; 20 - 25: 0,0439; 25 - 30: 0,0434; 30 - 35: 0,0426; 35 - 40: 0,0422; 40 - 45: 0,0417; 45 - 50: 0,0414; </v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
@@ -2283,11 +2328,11 @@
       </c>
       <c r="N13" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">[0 - 5: 120; 5 - 10: 79.08; 10 - 15: 89.76; 15 - 20: 86.28; 20 - 25: 0; 25 - 30: 0; 30 - 35: 0; 35 - 40: 0; 40 - 45: 0; 45 - 50: 0; 50 - 100: 0; </v>
+        <v xml:space="preserve">[0 - 5: 120; 5 - 10: 79,08; 10 - 15: 89,76; 15 - 20: 86,28; 20 - 25: 0; 25 - 30: 0; 30 - 35: 0; 35 - 40: 0; 40 - 45: 0; 45 - 50: 0; 50 - 100: 0; </v>
       </c>
       <c r="O13" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">[0 - 5: 0.0463; 5 - 10: 0.0448; 10 - 15: 0.0417; 15 - 20: 0.0401; 20 - 25: 0.0439; 25 - 30: 0.0434; 30 - 35: 0.0426; 35 - 40: 0.0422; 40 - 45: 0.0417; 45 - 50: 0.0414; 50 - 100: 0.0411; </v>
+        <v xml:space="preserve">[0 - 5: 0,0463; 5 - 10: 0,0448; 10 - 15: 0,0417; 15 - 20: 0,0401; 20 - 25: 0,0439; 25 - 30: 0,0434; 30 - 35: 0,0426; 35 - 40: 0,0422; 40 - 45: 0,0417; 45 - 50: 0,0414; 50 - 100: 0,0411; </v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
@@ -2305,11 +2350,11 @@
       </c>
       <c r="N14" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">[0 - 5: 120; 5 - 10: 79.08; 10 - 15: 89.76; 15 - 20: 86.28; 20 - 25: 0; 25 - 30: 0; 30 - 35: 0; 35 - 40: 0; 40 - 45: 0; 45 - 50: 0; 50 - 100: 0; 100 - 150: 0; </v>
+        <v xml:space="preserve">[0 - 5: 120; 5 - 10: 79,08; 10 - 15: 89,76; 15 - 20: 86,28; 20 - 25: 0; 25 - 30: 0; 30 - 35: 0; 35 - 40: 0; 40 - 45: 0; 45 - 50: 0; 50 - 100: 0; 100 - 150: 0; </v>
       </c>
       <c r="O14" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">[0 - 5: 0.0463; 5 - 10: 0.0448; 10 - 15: 0.0417; 15 - 20: 0.0401; 20 - 25: 0.0439; 25 - 30: 0.0434; 30 - 35: 0.0426; 35 - 40: 0.0422; 40 - 45: 0.0417; 45 - 50: 0.0414; 50 - 100: 0.0411; 100 - 150: 0.0399; </v>
+        <v xml:space="preserve">[0 - 5: 0,0463; 5 - 10: 0,0448; 10 - 15: 0,0417; 15 - 20: 0,0401; 20 - 25: 0,0439; 25 - 30: 0,0434; 30 - 35: 0,0426; 35 - 40: 0,0422; 40 - 45: 0,0417; 45 - 50: 0,0414; 50 - 100: 0,0411; 100 - 150: 0,0399; </v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
@@ -2327,11 +2372,11 @@
       </c>
       <c r="N15" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">[0 - 5: 120; 5 - 10: 79.08; 10 - 15: 89.76; 15 - 20: 86.28; 20 - 25: 0; 25 - 30: 0; 30 - 35: 0; 35 - 40: 0; 40 - 45: 0; 45 - 50: 0; 50 - 100: 0; 100 - 150: 0; 150 - 200: 0; </v>
+        <v xml:space="preserve">[0 - 5: 120; 5 - 10: 79,08; 10 - 15: 89,76; 15 - 20: 86,28; 20 - 25: 0; 25 - 30: 0; 30 - 35: 0; 35 - 40: 0; 40 - 45: 0; 45 - 50: 0; 50 - 100: 0; 100 - 150: 0; 150 - 200: 0; </v>
       </c>
       <c r="O15" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">[0 - 5: 0.0463; 5 - 10: 0.0448; 10 - 15: 0.0417; 15 - 20: 0.0401; 20 - 25: 0.0439; 25 - 30: 0.0434; 30 - 35: 0.0426; 35 - 40: 0.0422; 40 - 45: 0.0417; 45 - 50: 0.0414; 50 - 100: 0.0411; 100 - 150: 0.0399; 150 - 200: 0.0392; </v>
+        <v xml:space="preserve">[0 - 5: 0,0463; 5 - 10: 0,0448; 10 - 15: 0,0417; 15 - 20: 0,0401; 20 - 25: 0,0439; 25 - 30: 0,0434; 30 - 35: 0,0426; 35 - 40: 0,0422; 40 - 45: 0,0417; 45 - 50: 0,0414; 50 - 100: 0,0411; 100 - 150: 0,0399; 150 - 200: 0,0392; </v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
@@ -2349,11 +2394,11 @@
       </c>
       <c r="N16" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">[0 - 5: 120; 5 - 10: 79.08; 10 - 15: 89.76; 15 - 20: 86.28; 20 - 25: 0; 25 - 30: 0; 30 - 35: 0; 35 - 40: 0; 40 - 45: 0; 45 - 50: 0; 50 - 100: 0; 100 - 150: 0; 150 - 200: 0; 200 - 250: 340.08; </v>
+        <v xml:space="preserve">[0 - 5: 120; 5 - 10: 79,08; 10 - 15: 89,76; 15 - 20: 86,28; 20 - 25: 0; 25 - 30: 0; 30 - 35: 0; 35 - 40: 0; 40 - 45: 0; 45 - 50: 0; 50 - 100: 0; 100 - 150: 0; 150 - 200: 0; 200 - 250: 340,08; </v>
       </c>
       <c r="O16" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">[0 - 5: 0.0463; 5 - 10: 0.0448; 10 - 15: 0.0417; 15 - 20: 0.0401; 20 - 25: 0.0439; 25 - 30: 0.0434; 30 - 35: 0.0426; 35 - 40: 0.0422; 40 - 45: 0.0417; 45 - 50: 0.0414; 50 - 100: 0.0411; 100 - 150: 0.0399; 150 - 200: 0.0392; 200 - 250: 0.0379; </v>
+        <v xml:space="preserve">[0 - 5: 0,0463; 5 - 10: 0,0448; 10 - 15: 0,0417; 15 - 20: 0,0401; 20 - 25: 0,0439; 25 - 30: 0,0434; 30 - 35: 0,0426; 35 - 40: 0,0422; 40 - 45: 0,0417; 45 - 50: 0,0414; 50 - 100: 0,0411; 100 - 150: 0,0399; 150 - 200: 0,0392; 200 - 250: 0,0379; </v>
       </c>
     </row>
     <row r="17" spans="9:15" x14ac:dyDescent="0.25">
@@ -2371,11 +2416,11 @@
       </c>
       <c r="N17" t="str">
         <f t="shared" si="1"/>
-        <v xml:space="preserve">[0 - 5: 120; 5 - 10: 79.08; 10 - 15: 89.76; 15 - 20: 86.28; 20 - 25: 0; 25 - 30: 0; 30 - 35: 0; 35 - 40: 0; 40 - 45: 0; 45 - 50: 0; 50 - 100: 0; 100 - 150: 0; 150 - 200: 0; 200 - 250: 340.08; 250 - 500: 388.92; </v>
+        <v xml:space="preserve">[0 - 5: 120; 5 - 10: 79,08; 10 - 15: 89,76; 15 - 20: 86,28; 20 - 25: 0; 25 - 30: 0; 30 - 35: 0; 35 - 40: 0; 40 - 45: 0; 45 - 50: 0; 50 - 100: 0; 100 - 150: 0; 150 - 200: 0; 200 - 250: 340,08; 250 - 500: 388,92; </v>
       </c>
       <c r="O17" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">[0 - 5: 0.0463; 5 - 10: 0.0448; 10 - 15: 0.0417; 15 - 20: 0.0401; 20 - 25: 0.0439; 25 - 30: 0.0434; 30 - 35: 0.0426; 35 - 40: 0.0422; 40 - 45: 0.0417; 45 - 50: 0.0414; 50 - 100: 0.0411; 100 - 150: 0.0399; 150 - 200: 0.0392; 200 - 250: 0.0379; 250 - 500: 0.0379; </v>
+        <v xml:space="preserve">[0 - 5: 0,0463; 5 - 10: 0,0448; 10 - 15: 0,0417; 15 - 20: 0,0401; 20 - 25: 0,0439; 25 - 30: 0,0434; 30 - 35: 0,0426; 35 - 40: 0,0422; 40 - 45: 0,0417; 45 - 50: 0,0414; 50 - 100: 0,0411; 100 - 150: 0,0399; 150 - 200: 0,0392; 200 - 250: 0,0379; 250 - 500: 0,0379; </v>
       </c>
     </row>
     <row r="19" spans="9:15" x14ac:dyDescent="0.25">
@@ -2425,7 +2470,7 @@
       </c>
       <c r="O21" t="str">
         <f>CONCATENATE(O20,I21, " - ",J21,": ",L21,"; ")</f>
-        <v xml:space="preserve">[0 - 5: 0.047; </v>
+        <v xml:space="preserve">[0 - 5: 0,047; </v>
       </c>
     </row>
     <row r="22" spans="9:15" x14ac:dyDescent="0.25">
@@ -2443,11 +2488,11 @@
       </c>
       <c r="N22" t="str">
         <f t="shared" ref="N22:N35" si="2">CONCATENATE(N21,I22, " - ",J22,": ",K22,"; ")</f>
-        <v xml:space="preserve">[0 - 5: 120; 5 - 10: 79.08; </v>
+        <v xml:space="preserve">[0 - 5: 120; 5 - 10: 79,08; </v>
       </c>
       <c r="O22" t="str">
         <f t="shared" ref="O22:O35" si="3">CONCATENATE(O21,I22, " - ",J22,": ",L22,"; ")</f>
-        <v xml:space="preserve">[0 - 5: 0.047; 5 - 10: 0.0446; </v>
+        <v xml:space="preserve">[0 - 5: 0,047; 5 - 10: 0,0446; </v>
       </c>
     </row>
     <row r="23" spans="9:15" x14ac:dyDescent="0.25">
@@ -2465,11 +2510,11 @@
       </c>
       <c r="N23" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">[0 - 5: 120; 5 - 10: 79.08; 10 - 15: 89.76; </v>
+        <v xml:space="preserve">[0 - 5: 120; 5 - 10: 79,08; 10 - 15: 89,76; </v>
       </c>
       <c r="O23" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">[0 - 5: 0.047; 5 - 10: 0.0446; 10 - 15: 0.0415; </v>
+        <v xml:space="preserve">[0 - 5: 0,047; 5 - 10: 0,0446; 10 - 15: 0,0415; </v>
       </c>
     </row>
     <row r="24" spans="9:15" x14ac:dyDescent="0.25">
@@ -2487,11 +2532,11 @@
       </c>
       <c r="N24" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">[0 - 5: 120; 5 - 10: 79.08; 10 - 15: 89.76; 15 - 20: 86.28; </v>
+        <v xml:space="preserve">[0 - 5: 120; 5 - 10: 79,08; 10 - 15: 89,76; 15 - 20: 86,28; </v>
       </c>
       <c r="O24" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">[0 - 5: 0.047; 5 - 10: 0.0446; 10 - 15: 0.0415; 15 - 20: 0.0399; </v>
+        <v xml:space="preserve">[0 - 5: 0,047; 5 - 10: 0,0446; 10 - 15: 0,0415; 15 - 20: 0,0399; </v>
       </c>
     </row>
     <row r="25" spans="9:15" x14ac:dyDescent="0.25">
@@ -2509,11 +2554,11 @@
       </c>
       <c r="N25" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">[0 - 5: 120; 5 - 10: 79.08; 10 - 15: 89.76; 15 - 20: 86.28; 20 - 25: 0; </v>
+        <v xml:space="preserve">[0 - 5: 120; 5 - 10: 79,08; 10 - 15: 89,76; 15 - 20: 86,28; 20 - 25: 0; </v>
       </c>
       <c r="O25" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">[0 - 5: 0.047; 5 - 10: 0.0446; 10 - 15: 0.0415; 15 - 20: 0.0399; 20 - 25: 0.0437; </v>
+        <v xml:space="preserve">[0 - 5: 0,047; 5 - 10: 0,0446; 10 - 15: 0,0415; 15 - 20: 0,0399; 20 - 25: 0,0437; </v>
       </c>
     </row>
     <row r="26" spans="9:15" x14ac:dyDescent="0.25">
@@ -2531,11 +2576,11 @@
       </c>
       <c r="N26" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">[0 - 5: 120; 5 - 10: 79.08; 10 - 15: 89.76; 15 - 20: 86.28; 20 - 25: 0; 25 - 30: 0; </v>
+        <v xml:space="preserve">[0 - 5: 120; 5 - 10: 79,08; 10 - 15: 89,76; 15 - 20: 86,28; 20 - 25: 0; 25 - 30: 0; </v>
       </c>
       <c r="O26" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">[0 - 5: 0.047; 5 - 10: 0.0446; 10 - 15: 0.0415; 15 - 20: 0.0399; 20 - 25: 0.0437; 25 - 30: 0.0432; </v>
+        <v xml:space="preserve">[0 - 5: 0,047; 5 - 10: 0,0446; 10 - 15: 0,0415; 15 - 20: 0,0399; 20 - 25: 0,0437; 25 - 30: 0,0432; </v>
       </c>
     </row>
     <row r="27" spans="9:15" x14ac:dyDescent="0.25">
@@ -2553,11 +2598,11 @@
       </c>
       <c r="N27" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">[0 - 5: 120; 5 - 10: 79.08; 10 - 15: 89.76; 15 - 20: 86.28; 20 - 25: 0; 25 - 30: 0; 30 - 35: 0; </v>
+        <v xml:space="preserve">[0 - 5: 120; 5 - 10: 79,08; 10 - 15: 89,76; 15 - 20: 86,28; 20 - 25: 0; 25 - 30: 0; 30 - 35: 0; </v>
       </c>
       <c r="O27" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">[0 - 5: 0.047; 5 - 10: 0.0446; 10 - 15: 0.0415; 15 - 20: 0.0399; 20 - 25: 0.0437; 25 - 30: 0.0432; 30 - 35: 0.0424; </v>
+        <v xml:space="preserve">[0 - 5: 0,047; 5 - 10: 0,0446; 10 - 15: 0,0415; 15 - 20: 0,0399; 20 - 25: 0,0437; 25 - 30: 0,0432; 30 - 35: 0,0424; </v>
       </c>
     </row>
     <row r="28" spans="9:15" x14ac:dyDescent="0.25">
@@ -2575,11 +2620,11 @@
       </c>
       <c r="N28" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">[0 - 5: 120; 5 - 10: 79.08; 10 - 15: 89.76; 15 - 20: 86.28; 20 - 25: 0; 25 - 30: 0; 30 - 35: 0; 35 - 40: 0; </v>
+        <v xml:space="preserve">[0 - 5: 120; 5 - 10: 79,08; 10 - 15: 89,76; 15 - 20: 86,28; 20 - 25: 0; 25 - 30: 0; 30 - 35: 0; 35 - 40: 0; </v>
       </c>
       <c r="O28" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">[0 - 5: 0.047; 5 - 10: 0.0446; 10 - 15: 0.0415; 15 - 20: 0.0399; 20 - 25: 0.0437; 25 - 30: 0.0432; 30 - 35: 0.0424; 35 - 40: 0.042; </v>
+        <v xml:space="preserve">[0 - 5: 0,047; 5 - 10: 0,0446; 10 - 15: 0,0415; 15 - 20: 0,0399; 20 - 25: 0,0437; 25 - 30: 0,0432; 30 - 35: 0,0424; 35 - 40: 0,042; </v>
       </c>
     </row>
     <row r="29" spans="9:15" x14ac:dyDescent="0.25">
@@ -2597,11 +2642,11 @@
       </c>
       <c r="N29" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">[0 - 5: 120; 5 - 10: 79.08; 10 - 15: 89.76; 15 - 20: 86.28; 20 - 25: 0; 25 - 30: 0; 30 - 35: 0; 35 - 40: 0; 40 - 45: 0; </v>
+        <v xml:space="preserve">[0 - 5: 120; 5 - 10: 79,08; 10 - 15: 89,76; 15 - 20: 86,28; 20 - 25: 0; 25 - 30: 0; 30 - 35: 0; 35 - 40: 0; 40 - 45: 0; </v>
       </c>
       <c r="O29" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">[0 - 5: 0.047; 5 - 10: 0.0446; 10 - 15: 0.0415; 15 - 20: 0.0399; 20 - 25: 0.0437; 25 - 30: 0.0432; 30 - 35: 0.0424; 35 - 40: 0.042; 40 - 45: 0.0415; </v>
+        <v xml:space="preserve">[0 - 5: 0,047; 5 - 10: 0,0446; 10 - 15: 0,0415; 15 - 20: 0,0399; 20 - 25: 0,0437; 25 - 30: 0,0432; 30 - 35: 0,0424; 35 - 40: 0,042; 40 - 45: 0,0415; </v>
       </c>
     </row>
     <row r="30" spans="9:15" x14ac:dyDescent="0.25">
@@ -2619,11 +2664,11 @@
       </c>
       <c r="N30" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">[0 - 5: 120; 5 - 10: 79.08; 10 - 15: 89.76; 15 - 20: 86.28; 20 - 25: 0; 25 - 30: 0; 30 - 35: 0; 35 - 40: 0; 40 - 45: 0; 45 - 50: 0; </v>
+        <v xml:space="preserve">[0 - 5: 120; 5 - 10: 79,08; 10 - 15: 89,76; 15 - 20: 86,28; 20 - 25: 0; 25 - 30: 0; 30 - 35: 0; 35 - 40: 0; 40 - 45: 0; 45 - 50: 0; </v>
       </c>
       <c r="O30" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">[0 - 5: 0.047; 5 - 10: 0.0446; 10 - 15: 0.0415; 15 - 20: 0.0399; 20 - 25: 0.0437; 25 - 30: 0.0432; 30 - 35: 0.0424; 35 - 40: 0.042; 40 - 45: 0.0415; 45 - 50: 0.0412; </v>
+        <v xml:space="preserve">[0 - 5: 0,047; 5 - 10: 0,0446; 10 - 15: 0,0415; 15 - 20: 0,0399; 20 - 25: 0,0437; 25 - 30: 0,0432; 30 - 35: 0,0424; 35 - 40: 0,042; 40 - 45: 0,0415; 45 - 50: 0,0412; </v>
       </c>
     </row>
     <row r="31" spans="9:15" x14ac:dyDescent="0.25">
@@ -2641,11 +2686,11 @@
       </c>
       <c r="N31" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">[0 - 5: 120; 5 - 10: 79.08; 10 - 15: 89.76; 15 - 20: 86.28; 20 - 25: 0; 25 - 30: 0; 30 - 35: 0; 35 - 40: 0; 40 - 45: 0; 45 - 50: 0; 50 - 100: 0; </v>
+        <v xml:space="preserve">[0 - 5: 120; 5 - 10: 79,08; 10 - 15: 89,76; 15 - 20: 86,28; 20 - 25: 0; 25 - 30: 0; 30 - 35: 0; 35 - 40: 0; 40 - 45: 0; 45 - 50: 0; 50 - 100: 0; </v>
       </c>
       <c r="O31" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">[0 - 5: 0.047; 5 - 10: 0.0446; 10 - 15: 0.0415; 15 - 20: 0.0399; 20 - 25: 0.0437; 25 - 30: 0.0432; 30 - 35: 0.0424; 35 - 40: 0.042; 40 - 45: 0.0415; 45 - 50: 0.0412; 50 - 100: 0.0409; </v>
+        <v xml:space="preserve">[0 - 5: 0,047; 5 - 10: 0,0446; 10 - 15: 0,0415; 15 - 20: 0,0399; 20 - 25: 0,0437; 25 - 30: 0,0432; 30 - 35: 0,0424; 35 - 40: 0,042; 40 - 45: 0,0415; 45 - 50: 0,0412; 50 - 100: 0,0409; </v>
       </c>
     </row>
     <row r="32" spans="9:15" x14ac:dyDescent="0.25">
@@ -2663,11 +2708,11 @@
       </c>
       <c r="N32" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">[0 - 5: 120; 5 - 10: 79.08; 10 - 15: 89.76; 15 - 20: 86.28; 20 - 25: 0; 25 - 30: 0; 30 - 35: 0; 35 - 40: 0; 40 - 45: 0; 45 - 50: 0; 50 - 100: 0; 100 - 150: 0; </v>
+        <v xml:space="preserve">[0 - 5: 120; 5 - 10: 79,08; 10 - 15: 89,76; 15 - 20: 86,28; 20 - 25: 0; 25 - 30: 0; 30 - 35: 0; 35 - 40: 0; 40 - 45: 0; 45 - 50: 0; 50 - 100: 0; 100 - 150: 0; </v>
       </c>
       <c r="O32" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">[0 - 5: 0.047; 5 - 10: 0.0446; 10 - 15: 0.0415; 15 - 20: 0.0399; 20 - 25: 0.0437; 25 - 30: 0.0432; 30 - 35: 0.0424; 35 - 40: 0.042; 40 - 45: 0.0415; 45 - 50: 0.0412; 50 - 100: 0.0409; 100 - 150: 0.0397; </v>
+        <v xml:space="preserve">[0 - 5: 0,047; 5 - 10: 0,0446; 10 - 15: 0,0415; 15 - 20: 0,0399; 20 - 25: 0,0437; 25 - 30: 0,0432; 30 - 35: 0,0424; 35 - 40: 0,042; 40 - 45: 0,0415; 45 - 50: 0,0412; 50 - 100: 0,0409; 100 - 150: 0,0397; </v>
       </c>
     </row>
     <row r="33" spans="9:15" x14ac:dyDescent="0.25">
@@ -2685,11 +2730,11 @@
       </c>
       <c r="N33" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">[0 - 5: 120; 5 - 10: 79.08; 10 - 15: 89.76; 15 - 20: 86.28; 20 - 25: 0; 25 - 30: 0; 30 - 35: 0; 35 - 40: 0; 40 - 45: 0; 45 - 50: 0; 50 - 100: 0; 100 - 150: 0; 150 - 200: 0; </v>
+        <v xml:space="preserve">[0 - 5: 120; 5 - 10: 79,08; 10 - 15: 89,76; 15 - 20: 86,28; 20 - 25: 0; 25 - 30: 0; 30 - 35: 0; 35 - 40: 0; 40 - 45: 0; 45 - 50: 0; 50 - 100: 0; 100 - 150: 0; 150 - 200: 0; </v>
       </c>
       <c r="O33" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">[0 - 5: 0.047; 5 - 10: 0.0446; 10 - 15: 0.0415; 15 - 20: 0.0399; 20 - 25: 0.0437; 25 - 30: 0.0432; 30 - 35: 0.0424; 35 - 40: 0.042; 40 - 45: 0.0415; 45 - 50: 0.0412; 50 - 100: 0.0409; 100 - 150: 0.0397; 150 - 200: 0.039; </v>
+        <v xml:space="preserve">[0 - 5: 0,047; 5 - 10: 0,0446; 10 - 15: 0,0415; 15 - 20: 0,0399; 20 - 25: 0,0437; 25 - 30: 0,0432; 30 - 35: 0,0424; 35 - 40: 0,042; 40 - 45: 0,0415; 45 - 50: 0,0412; 50 - 100: 0,0409; 100 - 150: 0,0397; 150 - 200: 0,039; </v>
       </c>
     </row>
     <row r="34" spans="9:15" x14ac:dyDescent="0.25">
@@ -2707,11 +2752,11 @@
       </c>
       <c r="N34" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">[0 - 5: 120; 5 - 10: 79.08; 10 - 15: 89.76; 15 - 20: 86.28; 20 - 25: 0; 25 - 30: 0; 30 - 35: 0; 35 - 40: 0; 40 - 45: 0; 45 - 50: 0; 50 - 100: 0; 100 - 150: 0; 150 - 200: 0; 200 - 250: 340.08; </v>
+        <v xml:space="preserve">[0 - 5: 120; 5 - 10: 79,08; 10 - 15: 89,76; 15 - 20: 86,28; 20 - 25: 0; 25 - 30: 0; 30 - 35: 0; 35 - 40: 0; 40 - 45: 0; 45 - 50: 0; 50 - 100: 0; 100 - 150: 0; 150 - 200: 0; 200 - 250: 340,08; </v>
       </c>
       <c r="O34" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">[0 - 5: 0.047; 5 - 10: 0.0446; 10 - 15: 0.0415; 15 - 20: 0.0399; 20 - 25: 0.0437; 25 - 30: 0.0432; 30 - 35: 0.0424; 35 - 40: 0.042; 40 - 45: 0.0415; 45 - 50: 0.0412; 50 - 100: 0.0409; 100 - 150: 0.0397; 150 - 200: 0.039; 200 - 250: 0.0377; </v>
+        <v xml:space="preserve">[0 - 5: 0,047; 5 - 10: 0,0446; 10 - 15: 0,0415; 15 - 20: 0,0399; 20 - 25: 0,0437; 25 - 30: 0,0432; 30 - 35: 0,0424; 35 - 40: 0,042; 40 - 45: 0,0415; 45 - 50: 0,0412; 50 - 100: 0,0409; 100 - 150: 0,0397; 150 - 200: 0,039; 200 - 250: 0,0377; </v>
       </c>
     </row>
     <row r="35" spans="9:15" x14ac:dyDescent="0.25">
@@ -2729,11 +2774,11 @@
       </c>
       <c r="N35" t="str">
         <f t="shared" si="2"/>
-        <v xml:space="preserve">[0 - 5: 120; 5 - 10: 79.08; 10 - 15: 89.76; 15 - 20: 86.28; 20 - 25: 0; 25 - 30: 0; 30 - 35: 0; 35 - 40: 0; 40 - 45: 0; 45 - 50: 0; 50 - 100: 0; 100 - 150: 0; 150 - 200: 0; 200 - 250: 340.08; 250 - 500: 388.92; </v>
+        <v xml:space="preserve">[0 - 5: 120; 5 - 10: 79,08; 10 - 15: 89,76; 15 - 20: 86,28; 20 - 25: 0; 25 - 30: 0; 30 - 35: 0; 35 - 40: 0; 40 - 45: 0; 45 - 50: 0; 50 - 100: 0; 100 - 150: 0; 150 - 200: 0; 200 - 250: 340,08; 250 - 500: 388,92; </v>
       </c>
       <c r="O35" t="str">
         <f t="shared" si="3"/>
-        <v xml:space="preserve">[0 - 5: 0.047; 5 - 10: 0.0446; 10 - 15: 0.0415; 15 - 20: 0.0399; 20 - 25: 0.0437; 25 - 30: 0.0432; 30 - 35: 0.0424; 35 - 40: 0.042; 40 - 45: 0.0415; 45 - 50: 0.0412; 50 - 100: 0.0409; 100 - 150: 0.0397; 150 - 200: 0.039; 200 - 250: 0.0377; 250 - 500: 0.0377; </v>
+        <v xml:space="preserve">[0 - 5: 0,047; 5 - 10: 0,0446; 10 - 15: 0,0415; 15 - 20: 0,0399; 20 - 25: 0,0437; 25 - 30: 0,0432; 30 - 35: 0,0424; 35 - 40: 0,042; 40 - 45: 0,0415; 45 - 50: 0,0412; 50 - 100: 0,0409; 100 - 150: 0,0397; 150 - 200: 0,039; 200 - 250: 0,0377; 250 - 500: 0,0377; </v>
       </c>
     </row>
     <row r="39" spans="9:15" x14ac:dyDescent="0.25">
@@ -2769,11 +2814,11 @@
       </c>
       <c r="N41" t="str">
         <f t="shared" ref="N41:N50" si="4">CONCATENATE(N40,I41, " - ",J41,": ",K41,"; ")</f>
-        <v xml:space="preserve">[0.5 - 1.5: 109.68; </v>
+        <v xml:space="preserve">[0,5 - 1,5: 109,68; </v>
       </c>
       <c r="O41" t="str">
         <f t="shared" ref="O41:O50" si="5">CONCATENATE(O40,I41, " - ",J41,": ",L41,"; ")</f>
-        <v xml:space="preserve">[0.5 - 1.5: 0.2464; </v>
+        <v xml:space="preserve">[0,5 - 1,5: 0,2464; </v>
       </c>
     </row>
     <row r="42" spans="9:15" x14ac:dyDescent="0.25">
@@ -2792,11 +2837,11 @@
       </c>
       <c r="N42" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">[0.5 - 1.5: 109.68; 1.5 - 2: 70.08; </v>
+        <v xml:space="preserve">[0,5 - 1,5: 109,68; 1,5 - 2: 70,08; </v>
       </c>
       <c r="O42" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">[0.5 - 1.5: 0.2464; 1.5 - 2: 0.2276; </v>
+        <v xml:space="preserve">[0,5 - 1,5: 0,2464; 1,5 - 2: 0,2276; </v>
       </c>
     </row>
     <row r="43" spans="9:15" x14ac:dyDescent="0.25">
@@ -2815,11 +2860,11 @@
       </c>
       <c r="N43" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">[0.5 - 1.5: 109.68; 1.5 - 2: 70.08; 2 - 2.5: 67.08; </v>
+        <v xml:space="preserve">[0,5 - 1,5: 109,68; 1,5 - 2: 70,08; 2 - 2,5: 67,08; </v>
       </c>
       <c r="O43" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">[0.5 - 1.5: 0.2464; 1.5 - 2: 0.2276; 2 - 2.5: 0.2207; </v>
+        <v xml:space="preserve">[0,5 - 1,5: 0,2464; 1,5 - 2: 0,2276; 2 - 2,5: 0,2207; </v>
       </c>
     </row>
     <row r="44" spans="9:15" x14ac:dyDescent="0.25">
@@ -2838,11 +2883,11 @@
       </c>
       <c r="N44" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">[0.5 - 1.5: 109.68; 1.5 - 2: 70.08; 2 - 2.5: 67.08; 2.5 - 3: 66; </v>
+        <v xml:space="preserve">[0,5 - 1,5: 109,68; 1,5 - 2: 70,08; 2 - 2,5: 67,08; 2,5 - 3: 66; </v>
       </c>
       <c r="O44" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">[0.5 - 1.5: 0.2464; 1.5 - 2: 0.2276; 2 - 2.5: 0.2207; 2.5 - 3: 0.2198; </v>
+        <v xml:space="preserve">[0,5 - 1,5: 0,2464; 1,5 - 2: 0,2276; 2 - 2,5: 0,2207; 2,5 - 3: 0,2198; </v>
       </c>
     </row>
     <row r="45" spans="9:15" x14ac:dyDescent="0.25">
@@ -2862,11 +2907,11 @@
       </c>
       <c r="N45" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">[0.5 - 1.5: 109.68; 1.5 - 2: 70.08; 2 - 2.5: 67.08; 2.5 - 3: 66; 3 - 4: 75.36; </v>
+        <v xml:space="preserve">[0,5 - 1,5: 109,68; 1,5 - 2: 70,08; 2 - 2,5: 67,08; 2,5 - 3: 66; 3 - 4: 75,36; </v>
       </c>
       <c r="O45" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">[0.5 - 1.5: 0.2464; 1.5 - 2: 0.2276; 2 - 2.5: 0.2207; 2.5 - 3: 0.2198; 3 - 4: 0.2146; </v>
+        <v xml:space="preserve">[0,5 - 1,5: 0,2464; 1,5 - 2: 0,2276; 2 - 2,5: 0,2207; 2,5 - 3: 0,2198; 3 - 4: 0,2146; </v>
       </c>
     </row>
     <row r="46" spans="9:15" x14ac:dyDescent="0.25">
@@ -2885,11 +2930,11 @@
       </c>
       <c r="N46" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">[0.5 - 1.5: 109.68; 1.5 - 2: 70.08; 2 - 2.5: 67.08; 2.5 - 3: 66; 3 - 4: 75.36; 4 - 4.5: 66; </v>
+        <v xml:space="preserve">[0,5 - 1,5: 109,68; 1,5 - 2: 70,08; 2 - 2,5: 67,08; 2,5 - 3: 66; 3 - 4: 75,36; 4 - 4,5: 66; </v>
       </c>
       <c r="O46" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">[0.5 - 1.5: 0.2464; 1.5 - 2: 0.2276; 2 - 2.5: 0.2207; 2.5 - 3: 0.2198; 3 - 4: 0.2146; 4 - 4.5: 0.2176; </v>
+        <v xml:space="preserve">[0,5 - 1,5: 0,2464; 1,5 - 2: 0,2276; 2 - 2,5: 0,2207; 2,5 - 3: 0,2198; 3 - 4: 0,2146; 4 - 4,5: 0,2176; </v>
       </c>
     </row>
     <row r="47" spans="9:15" x14ac:dyDescent="0.25">
@@ -2908,11 +2953,11 @@
       </c>
       <c r="N47" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">[0.5 - 1.5: 109.68; 1.5 - 2: 70.08; 2 - 2.5: 67.08; 2.5 - 3: 66; 3 - 4: 75.36; 4 - 4.5: 66; 4.5 - 5: 65.88; </v>
+        <v xml:space="preserve">[0,5 - 1,5: 109,68; 1,5 - 2: 70,08; 2 - 2,5: 67,08; 2,5 - 3: 66; 3 - 4: 75,36; 4 - 4,5: 66; 4,5 - 5: 65,88; </v>
       </c>
       <c r="O47" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">[0.5 - 1.5: 0.2464; 1.5 - 2: 0.2276; 2 - 2.5: 0.2207; 2.5 - 3: 0.2198; 3 - 4: 0.2146; 4 - 4.5: 0.2176; 4.5 - 5: 0.2166; </v>
+        <v xml:space="preserve">[0,5 - 1,5: 0,2464; 1,5 - 2: 0,2276; 2 - 2,5: 0,2207; 2,5 - 3: 0,2198; 3 - 4: 0,2146; 4 - 4,5: 0,2176; 4,5 - 5: 0,2166; </v>
       </c>
     </row>
     <row r="48" spans="9:15" x14ac:dyDescent="0.25">
@@ -2931,11 +2976,11 @@
       </c>
       <c r="N48" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">[0.5 - 1.5: 109.68; 1.5 - 2: 70.08; 2 - 2.5: 67.08; 2.5 - 3: 66; 3 - 4: 75.36; 4 - 4.5: 66; 4.5 - 5: 65.88; 5 - 6: 61.56; </v>
+        <v xml:space="preserve">[0,5 - 1,5: 109,68; 1,5 - 2: 70,08; 2 - 2,5: 67,08; 2,5 - 3: 66; 3 - 4: 75,36; 4 - 4,5: 66; 4,5 - 5: 65,88; 5 - 6: 61,56; </v>
       </c>
       <c r="O48" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">[0.5 - 1.5: 0.2464; 1.5 - 2: 0.2276; 2 - 2.5: 0.2207; 2.5 - 3: 0.2198; 3 - 4: 0.2146; 4 - 4.5: 0.2176; 4.5 - 5: 0.2166; 5 - 6: 0.2166; </v>
+        <v xml:space="preserve">[0,5 - 1,5: 0,2464; 1,5 - 2: 0,2276; 2 - 2,5: 0,2207; 2,5 - 3: 0,2198; 3 - 4: 0,2146; 4 - 4,5: 0,2176; 4,5 - 5: 0,2166; 5 - 6: 0,2166; </v>
       </c>
     </row>
     <row r="49" spans="6:15" x14ac:dyDescent="0.25">
@@ -2954,11 +2999,11 @@
       </c>
       <c r="N49" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">[0.5 - 1.5: 109.68; 1.5 - 2: 70.08; 2 - 2.5: 67.08; 2.5 - 3: 66; 3 - 4: 75.36; 4 - 4.5: 66; 4.5 - 5: 65.88; 5 - 6: 61.56; 6 - 7: 57.12; </v>
+        <v xml:space="preserve">[0,5 - 1,5: 109,68; 1,5 - 2: 70,08; 2 - 2,5: 67,08; 2,5 - 3: 66; 3 - 4: 75,36; 4 - 4,5: 66; 4,5 - 5: 65,88; 5 - 6: 61,56; 6 - 7: 57,12; </v>
       </c>
       <c r="O49" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">[0.5 - 1.5: 0.2464; 1.5 - 2: 0.2276; 2 - 2.5: 0.2207; 2.5 - 3: 0.2198; 3 - 4: 0.2146; 4 - 4.5: 0.2176; 4.5 - 5: 0.2166; 5 - 6: 0.2166; 6 - 7: 0.2162; </v>
+        <v xml:space="preserve">[0,5 - 1,5: 0,2464; 1,5 - 2: 0,2276; 2 - 2,5: 0,2207; 2,5 - 3: 0,2198; 3 - 4: 0,2146; 4 - 4,5: 0,2176; 4,5 - 5: 0,2166; 5 - 6: 0,2166; 6 - 7: 0,2162; </v>
       </c>
     </row>
     <row r="50" spans="6:15" x14ac:dyDescent="0.25">
@@ -2977,11 +3022,11 @@
       </c>
       <c r="N50" t="str">
         <f t="shared" si="4"/>
-        <v xml:space="preserve">[0.5 - 1.5: 109.68; 1.5 - 2: 70.08; 2 - 2.5: 67.08; 2.5 - 3: 66; 3 - 4: 75.36; 4 - 4.5: 66; 4.5 - 5: 65.88; 5 - 6: 61.56; 6 - 7: 57.12; 7 - 100: 66.84; </v>
+        <v xml:space="preserve">[0,5 - 1,5: 109,68; 1,5 - 2: 70,08; 2 - 2,5: 67,08; 2,5 - 3: 66; 3 - 4: 75,36; 4 - 4,5: 66; 4,5 - 5: 65,88; 5 - 6: 61,56; 6 - 7: 57,12; 7 - 100: 66,84; </v>
       </c>
       <c r="O50" t="str">
         <f t="shared" si="5"/>
-        <v xml:space="preserve">[0.5 - 1.5: 0.2464; 1.5 - 2: 0.2276; 2 - 2.5: 0.2207; 2.5 - 3: 0.2198; 3 - 4: 0.2146; 4 - 4.5: 0.2176; 4.5 - 5: 0.2166; 5 - 6: 0.2166; 6 - 7: 0.2162; 7 - 100: 0.2154; </v>
+        <v xml:space="preserve">[0,5 - 1,5: 0,2464; 1,5 - 2: 0,2276; 2 - 2,5: 0,2207; 2,5 - 3: 0,2198; 3 - 4: 0,2146; 4 - 4,5: 0,2176; 4,5 - 5: 0,2166; 5 - 6: 0,2166; 6 - 7: 0,2162; 7 - 100: 0,2154; </v>
       </c>
     </row>
     <row r="52" spans="6:15" x14ac:dyDescent="0.25">
@@ -3018,11 +3063,11 @@
       </c>
       <c r="N54" t="str">
         <f t="shared" ref="N54:N63" si="6">CONCATENATE(N53,I54, " - ",J54,": ",K54,"; ")</f>
-        <v xml:space="preserve">[0.5 - 1.5: 109.68; </v>
+        <v xml:space="preserve">[0,5 - 1,5: 109,68; </v>
       </c>
       <c r="O54" t="str">
         <f t="shared" ref="O54:O63" si="7">CONCATENATE(O53,I54, " - ",J54,": ",L54,"; ")</f>
-        <v xml:space="preserve">[0.5 - 1.5: 0.2424; </v>
+        <v xml:space="preserve">[0,5 - 1,5: 0,2424; </v>
       </c>
     </row>
     <row r="55" spans="6:15" x14ac:dyDescent="0.25">
@@ -3043,11 +3088,11 @@
       </c>
       <c r="N55" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">[0.5 - 1.5: 109.68; 1.5 - 2: 70.08; </v>
+        <v xml:space="preserve">[0,5 - 1,5: 109,68; 1,5 - 2: 70,08; </v>
       </c>
       <c r="O55" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">[0.5 - 1.5: 0.2424; 1.5 - 2: 0.2278; </v>
+        <v xml:space="preserve">[0,5 - 1,5: 0,2424; 1,5 - 2: 0,2278; </v>
       </c>
     </row>
     <row r="56" spans="6:15" x14ac:dyDescent="0.25">
@@ -3068,11 +3113,11 @@
       </c>
       <c r="N56" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">[0.5 - 1.5: 109.68; 1.5 - 2: 70.08; 2 - 2.5: 67.08; </v>
+        <v xml:space="preserve">[0,5 - 1,5: 109,68; 1,5 - 2: 70,08; 2 - 2,5: 67,08; </v>
       </c>
       <c r="O56" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">[0.5 - 1.5: 0.2424; 1.5 - 2: 0.2278; 2 - 2.5: 0.2209; </v>
+        <v xml:space="preserve">[0,5 - 1,5: 0,2424; 1,5 - 2: 0,2278; 2 - 2,5: 0,2209; </v>
       </c>
     </row>
     <row r="57" spans="6:15" x14ac:dyDescent="0.25">
@@ -3093,11 +3138,11 @@
       </c>
       <c r="N57" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">[0.5 - 1.5: 109.68; 1.5 - 2: 70.08; 2 - 2.5: 67.08; 2.5 - 3: 66; </v>
+        <v xml:space="preserve">[0,5 - 1,5: 109,68; 1,5 - 2: 70,08; 2 - 2,5: 67,08; 2,5 - 3: 66; </v>
       </c>
       <c r="O57" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">[0.5 - 1.5: 0.2424; 1.5 - 2: 0.2278; 2 - 2.5: 0.2209; 2.5 - 3: 0.22; </v>
+        <v xml:space="preserve">[0,5 - 1,5: 0,2424; 1,5 - 2: 0,2278; 2 - 2,5: 0,2209; 2,5 - 3: 0,22; </v>
       </c>
     </row>
     <row r="58" spans="6:15" x14ac:dyDescent="0.25">
@@ -3118,11 +3163,11 @@
       </c>
       <c r="N58" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">[0.5 - 1.5: 109.68; 1.5 - 2: 70.08; 2 - 2.5: 67.08; 2.5 - 3: 66; 3 - 4: 75.36; </v>
+        <v xml:space="preserve">[0,5 - 1,5: 109,68; 1,5 - 2: 70,08; 2 - 2,5: 67,08; 2,5 - 3: 66; 3 - 4: 75,36; </v>
       </c>
       <c r="O58" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">[0.5 - 1.5: 0.2424; 1.5 - 2: 0.2278; 2 - 2.5: 0.2209; 2.5 - 3: 0.22; 3 - 4: 0.2148; </v>
+        <v xml:space="preserve">[0,5 - 1,5: 0,2424; 1,5 - 2: 0,2278; 2 - 2,5: 0,2209; 2,5 - 3: 0,22; 3 - 4: 0,2148; </v>
       </c>
     </row>
     <row r="59" spans="6:15" x14ac:dyDescent="0.25">
@@ -3143,11 +3188,11 @@
       </c>
       <c r="N59" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">[0.5 - 1.5: 109.68; 1.5 - 2: 70.08; 2 - 2.5: 67.08; 2.5 - 3: 66; 3 - 4: 75.36; 4 - 4.5: 66; </v>
+        <v xml:space="preserve">[0,5 - 1,5: 109,68; 1,5 - 2: 70,08; 2 - 2,5: 67,08; 2,5 - 3: 66; 3 - 4: 75,36; 4 - 4,5: 66; </v>
       </c>
       <c r="O59" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">[0.5 - 1.5: 0.2424; 1.5 - 2: 0.2278; 2 - 2.5: 0.2209; 2.5 - 3: 0.22; 3 - 4: 0.2148; 4 - 4.5: 0.2178; </v>
+        <v xml:space="preserve">[0,5 - 1,5: 0,2424; 1,5 - 2: 0,2278; 2 - 2,5: 0,2209; 2,5 - 3: 0,22; 3 - 4: 0,2148; 4 - 4,5: 0,2178; </v>
       </c>
     </row>
     <row r="60" spans="6:15" x14ac:dyDescent="0.25">
@@ -3168,11 +3213,11 @@
       </c>
       <c r="N60" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">[0.5 - 1.5: 109.68; 1.5 - 2: 70.08; 2 - 2.5: 67.08; 2.5 - 3: 66; 3 - 4: 75.36; 4 - 4.5: 66; 4.5 - 5: 65.88; </v>
+        <v xml:space="preserve">[0,5 - 1,5: 109,68; 1,5 - 2: 70,08; 2 - 2,5: 67,08; 2,5 - 3: 66; 3 - 4: 75,36; 4 - 4,5: 66; 4,5 - 5: 65,88; </v>
       </c>
       <c r="O60" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">[0.5 - 1.5: 0.2424; 1.5 - 2: 0.2278; 2 - 2.5: 0.2209; 2.5 - 3: 0.22; 3 - 4: 0.2148; 4 - 4.5: 0.2178; 4.5 - 5: 0.2168; </v>
+        <v xml:space="preserve">[0,5 - 1,5: 0,2424; 1,5 - 2: 0,2278; 2 - 2,5: 0,2209; 2,5 - 3: 0,22; 3 - 4: 0,2148; 4 - 4,5: 0,2178; 4,5 - 5: 0,2168; </v>
       </c>
     </row>
     <row r="61" spans="6:15" x14ac:dyDescent="0.25">
@@ -3193,11 +3238,11 @@
       </c>
       <c r="N61" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">[0.5 - 1.5: 109.68; 1.5 - 2: 70.08; 2 - 2.5: 67.08; 2.5 - 3: 66; 3 - 4: 75.36; 4 - 4.5: 66; 4.5 - 5: 65.88; 5 - 6: 61.56; </v>
+        <v xml:space="preserve">[0,5 - 1,5: 109,68; 1,5 - 2: 70,08; 2 - 2,5: 67,08; 2,5 - 3: 66; 3 - 4: 75,36; 4 - 4,5: 66; 4,5 - 5: 65,88; 5 - 6: 61,56; </v>
       </c>
       <c r="O61" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">[0.5 - 1.5: 0.2424; 1.5 - 2: 0.2278; 2 - 2.5: 0.2209; 2.5 - 3: 0.22; 3 - 4: 0.2148; 4 - 4.5: 0.2178; 4.5 - 5: 0.2168; 5 - 6: 0.2168; </v>
+        <v xml:space="preserve">[0,5 - 1,5: 0,2424; 1,5 - 2: 0,2278; 2 - 2,5: 0,2209; 2,5 - 3: 0,22; 3 - 4: 0,2148; 4 - 4,5: 0,2178; 4,5 - 5: 0,2168; 5 - 6: 0,2168; </v>
       </c>
     </row>
     <row r="62" spans="6:15" x14ac:dyDescent="0.25">
@@ -3218,11 +3263,11 @@
       </c>
       <c r="N62" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">[0.5 - 1.5: 109.68; 1.5 - 2: 70.08; 2 - 2.5: 67.08; 2.5 - 3: 66; 3 - 4: 75.36; 4 - 4.5: 66; 4.5 - 5: 65.88; 5 - 6: 61.56; 6 - 7: 57.12; </v>
+        <v xml:space="preserve">[0,5 - 1,5: 109,68; 1,5 - 2: 70,08; 2 - 2,5: 67,08; 2,5 - 3: 66; 3 - 4: 75,36; 4 - 4,5: 66; 4,5 - 5: 65,88; 5 - 6: 61,56; 6 - 7: 57,12; </v>
       </c>
       <c r="O62" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">[0.5 - 1.5: 0.2424; 1.5 - 2: 0.2278; 2 - 2.5: 0.2209; 2.5 - 3: 0.22; 3 - 4: 0.2148; 4 - 4.5: 0.2178; 4.5 - 5: 0.2168; 5 - 6: 0.2168; 6 - 7: 0.2164; </v>
+        <v xml:space="preserve">[0,5 - 1,5: 0,2424; 1,5 - 2: 0,2278; 2 - 2,5: 0,2209; 2,5 - 3: 0,22; 3 - 4: 0,2148; 4 - 4,5: 0,2178; 4,5 - 5: 0,2168; 5 - 6: 0,2168; 6 - 7: 0,2164; </v>
       </c>
     </row>
     <row r="63" spans="6:15" x14ac:dyDescent="0.25">
@@ -3243,11 +3288,11 @@
       </c>
       <c r="N63" t="str">
         <f t="shared" si="6"/>
-        <v xml:space="preserve">[0.5 - 1.5: 109.68; 1.5 - 2: 70.08; 2 - 2.5: 67.08; 2.5 - 3: 66; 3 - 4: 75.36; 4 - 4.5: 66; 4.5 - 5: 65.88; 5 - 6: 61.56; 6 - 7: 57.12; 7 - 100: 66.84; </v>
+        <v xml:space="preserve">[0,5 - 1,5: 109,68; 1,5 - 2: 70,08; 2 - 2,5: 67,08; 2,5 - 3: 66; 3 - 4: 75,36; 4 - 4,5: 66; 4,5 - 5: 65,88; 5 - 6: 61,56; 6 - 7: 57,12; 7 - 100: 66,84; </v>
       </c>
       <c r="O63" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">[0.5 - 1.5: 0.2424; 1.5 - 2: 0.2278; 2 - 2.5: 0.2209; 2.5 - 3: 0.22; 3 - 4: 0.2148; 4 - 4.5: 0.2178; 4.5 - 5: 0.2168; 5 - 6: 0.2168; 6 - 7: 0.2164; 7 - 100: 0.2156; </v>
+        <v xml:space="preserve">[0,5 - 1,5: 0,2424; 1,5 - 2: 0,2278; 2 - 2,5: 0,2209; 2,5 - 3: 0,22; 3 - 4: 0,2148; 4 - 4,5: 0,2178; 4,5 - 5: 0,2168; 5 - 6: 0,2168; 6 - 7: 0,2164; 7 - 100: 0,2156; </v>
       </c>
     </row>
     <row r="65" spans="9:15" x14ac:dyDescent="0.25">
@@ -3282,11 +3327,11 @@
       </c>
       <c r="N67" t="str">
         <f>CONCATENATE(N66,I67, " - ",J67,": ",K67,"; ")</f>
-        <v xml:space="preserve">[0 - 2.5: 76.08; </v>
+        <v xml:space="preserve">[0 - 2,5: 76,08; </v>
       </c>
       <c r="O67" t="str">
         <f>CONCATENATE(O66,I67, " - ",J67,": ",L67,"; ")</f>
-        <v xml:space="preserve">[0 - 2.5: 0.189; </v>
+        <v xml:space="preserve">[0 - 2,5: 0,189; </v>
       </c>
     </row>
     <row r="68" spans="9:15" x14ac:dyDescent="0.25">
@@ -3305,11 +3350,11 @@
       </c>
       <c r="N68" t="str">
         <f>CONCATENATE(N67,I68, " - ",J68,": ",K68,"; ")</f>
-        <v xml:space="preserve">[0 - 2.5: 76.08; 2.5 - 5: 118.92; </v>
+        <v xml:space="preserve">[0 - 2,5: 76,08; 2,5 - 5: 118,92; </v>
       </c>
       <c r="O68" t="str">
         <f>CONCATENATE(O67,I68, " - ",J68,": ",L68,"; ")</f>
-        <v xml:space="preserve">[0 - 2.5: 0.189; 2.5 - 5: 0.1648; </v>
+        <v xml:space="preserve">[0 - 2,5: 0,189; 2,5 - 5: 0,1648; </v>
       </c>
     </row>
     <row r="69" spans="9:15" x14ac:dyDescent="0.25">
@@ -3328,11 +3373,11 @@
       </c>
       <c r="N69" t="str">
         <f>CONCATENATE(N68,I69, " - ",J69,": ",K69,"; ")</f>
-        <v xml:space="preserve">[0 - 2.5: 76.08; 2.5 - 5: 118.92; 5 - 7.5: 46.32; </v>
+        <v xml:space="preserve">[0 - 2,5: 76,08; 2,5 - 5: 118,92; 5 - 7,5: 46,32; </v>
       </c>
       <c r="O69" t="str">
         <f>CONCATENATE(O68,I69, " - ",J69,": ",L69,"; ")</f>
-        <v xml:space="preserve">[0 - 2.5: 0.189; 2.5 - 5: 0.1648; 5 - 7.5: 0.1783; </v>
+        <v xml:space="preserve">[0 - 2,5: 0,189; 2,5 - 5: 0,1648; 5 - 7,5: 0,1783; </v>
       </c>
     </row>
     <row r="70" spans="9:15" x14ac:dyDescent="0.25">
@@ -3351,11 +3396,11 @@
       </c>
       <c r="N70" t="str">
         <f>CONCATENATE(N69,I70, " - ",J70,": ",K70,"; ")</f>
-        <v xml:space="preserve">[0 - 2.5: 76.08; 2.5 - 5: 118.92; 5 - 7.5: 46.32; 7.5 - 50: 119.04; </v>
+        <v xml:space="preserve">[0 - 2,5: 76,08; 2,5 - 5: 118,92; 5 - 7,5: 46,32; 7,5 - 50: 119,04; </v>
       </c>
       <c r="O70" t="str">
         <f>CONCATENATE(O69,I70, " - ",J70,": ",L70,"; ")</f>
-        <v xml:space="preserve">[0 - 2.5: 0.189; 2.5 - 5: 0.1648; 5 - 7.5: 0.1783; 7.5 - 50: 0.1648; </v>
+        <v xml:space="preserve">[0 - 2,5: 0,189; 2,5 - 5: 0,1648; 5 - 7,5: 0,1783; 7,5 - 50: 0,1648; </v>
       </c>
     </row>
     <row r="71" spans="9:15" x14ac:dyDescent="0.25">
@@ -3374,11 +3419,11 @@
       </c>
       <c r="N71" t="str">
         <f>CONCATENATE(N70,I71, " - ",J71,": ",K71,"; ")</f>
-        <v xml:space="preserve">[0 - 2.5: 76.08; 2.5 - 5: 118.92; 5 - 7.5: 46.32; 7.5 - 50: 119.04; 50 - 100: 119.16; </v>
+        <v xml:space="preserve">[0 - 2,5: 76,08; 2,5 - 5: 118,92; 5 - 7,5: 46,32; 7,5 - 50: 119,04; 50 - 100: 119,16; </v>
       </c>
       <c r="O71" t="str">
         <f>CONCATENATE(O70,I71, " - ",J71,": ",L71,"; ")</f>
-        <v xml:space="preserve">[0 - 2.5: 0.189; 2.5 - 5: 0.1648; 5 - 7.5: 0.1783; 7.5 - 50: 0.1648; 50 - 100: 0.1648; </v>
+        <v xml:space="preserve">[0 - 2,5: 0,189; 2,5 - 5: 0,1648; 5 - 7,5: 0,1783; 7,5 - 50: 0,1648; 50 - 100: 0,1648; </v>
       </c>
     </row>
     <row r="74" spans="9:15" x14ac:dyDescent="0.25">
@@ -3407,11 +3452,11 @@
       </c>
       <c r="N75" t="str">
         <f>CONCATENATE(N74,I75," - ",J75,": ",K75,IF(I76&gt;I75,"; ","]"))</f>
-        <v xml:space="preserve">[0 - 1.75: 60.45; </v>
+        <v xml:space="preserve">[0 - 1,75: 60,45; </v>
       </c>
       <c r="O75" t="str">
         <f>CONCATENATE(O74,I75, " - ",J75,": ",L75,IF(I76&gt;I75,"; ","]"))</f>
-        <v xml:space="preserve">[0 - 1.75: 0.2391; </v>
+        <v xml:space="preserve">[0 - 1,75: 0,2391; </v>
       </c>
     </row>
     <row r="76" spans="9:15" x14ac:dyDescent="0.25">
@@ -3429,11 +3474,11 @@
       </c>
       <c r="N76" t="str">
         <f>CONCATENATE(N75,I76," - ",J76,": ",K76,IF(I77&gt;I76,"; ","]"))</f>
-        <v xml:space="preserve">[0 - 1.75: 60.45; 1.75 - 2.75: 70.09; </v>
+        <v xml:space="preserve">[0 - 1,75: 60,45; 1,75 - 2,75: 70,09; </v>
       </c>
       <c r="O76" t="str">
         <f>CONCATENATE(O75,I76, " - ",J76,": ",L76,IF(I77&gt;I76,"; ","]"))</f>
-        <v xml:space="preserve">[0 - 1.75: 0.2391; 1.75 - 2.75: 0.2207; </v>
+        <v xml:space="preserve">[0 - 1,75: 0,2391; 1,75 - 2,75: 0,2207; </v>
       </c>
     </row>
     <row r="77" spans="9:15" x14ac:dyDescent="0.25">
@@ -3451,11 +3496,11 @@
       </c>
       <c r="N77" t="str">
         <f>CONCATENATE(N76,I77," - ",J77,": ",K77,IF(I78&gt;I77,"; ","]"))</f>
-        <v xml:space="preserve">[0 - 1.75: 60.45; 1.75 - 2.75: 70.09; 2.75 - 3.75: 78.3; </v>
+        <v xml:space="preserve">[0 - 1,75: 60,45; 1,75 - 2,75: 70,09; 2,75 - 3,75: 78,3; </v>
       </c>
       <c r="O77" t="str">
         <f>CONCATENATE(O76,I77, " - ",J77,": ",L77,IF(I78&gt;I77,"; ","]"))</f>
-        <v xml:space="preserve">[0 - 1.75: 0.2391; 1.75 - 2.75: 0.2207; 2.75 - 3.75: 0.2146; </v>
+        <v xml:space="preserve">[0 - 1,75: 0,2391; 1,75 - 2,75: 0,2207; 2,75 - 3,75: 0,2146; </v>
       </c>
     </row>
     <row r="78" spans="9:15" x14ac:dyDescent="0.25">
@@ -3473,11 +3518,11 @@
       </c>
       <c r="N78" t="str">
         <f>CONCATENATE(N77,I78," - ",J78,": ",K78,IF(I79&gt;I78,"; ","]"))</f>
-        <v xml:space="preserve">[0 - 1.75: 60.45; 1.75 - 2.75: 70.09; 2.75 - 3.75: 78.3; 3.75 - 4.75: 61.88; </v>
+        <v xml:space="preserve">[0 - 1,75: 60,45; 1,75 - 2,75: 70,09; 2,75 - 3,75: 78,3; 3,75 - 4,75: 61,88; </v>
       </c>
       <c r="O78" t="str">
         <f>CONCATENATE(O77,I78, " - ",J78,": ",L78,IF(I79&gt;I78,"; ","]"))</f>
-        <v xml:space="preserve">[0 - 1.75: 0.2391; 1.75 - 2.75: 0.2207; 2.75 - 3.75: 0.2146; 3.75 - 4.75: 0.2216; </v>
+        <v xml:space="preserve">[0 - 1,75: 0,2391; 1,75 - 2,75: 0,2207; 2,75 - 3,75: 0,2146; 3,75 - 4,75: 0,2216; </v>
       </c>
     </row>
     <row r="79" spans="9:15" x14ac:dyDescent="0.25">
@@ -3495,11 +3540,11 @@
       </c>
       <c r="N79" t="str">
         <f>CONCATENATE(N78,I79," - ",J79,": ",K79,IF(I82&gt;I79,"; ","]"))</f>
-        <v>[0 - 1.75: 60.45; 1.75 - 2.75: 70.09; 2.75 - 3.75: 78.3; 3.75 - 4.75: 61.88; 4.75 - 100: 61.88]</v>
+        <v>[0 - 1,75: 60,45; 1,75 - 2,75: 70,09; 2,75 - 3,75: 78,3; 3,75 - 4,75: 61,88; 4,75 - 100: 61,88]</v>
       </c>
       <c r="O79" t="str">
         <f>CONCATENATE(O78,I79, " - ",J79,": ",L79,IF(I82&gt;I79,"; ","]"))</f>
-        <v>[0 - 1.75: 0.2391; 1.75 - 2.75: 0.2207; 2.75 - 3.75: 0.2146; 3.75 - 4.75: 0.2216; 4.75 - 100: 0.2207]</v>
+        <v>[0 - 1,75: 0,2391; 1,75 - 2,75: 0,2207; 2,75 - 3,75: 0,2146; 3,75 - 4,75: 0,2216; 4,75 - 100: 0,2207]</v>
       </c>
     </row>
     <row r="81" spans="9:15" x14ac:dyDescent="0.25">
@@ -3528,11 +3573,11 @@
       </c>
       <c r="N82" t="str">
         <f>CONCATENATE(N81,I82," - ",J82,": ",K82,IF(I83&gt;I82,"; ","]"))</f>
-        <v>[0 - 100: 91.51]</v>
+        <v>[0 - 100: 91,51]</v>
       </c>
       <c r="O82" t="str">
         <f>CONCATENATE(O81,I82, " - ",J82,": ",L82,IF(I83&gt;I82,"; ","]"))</f>
-        <v>[0 - 100: 0.1958]</v>
+        <v>[0 - 100: 0,1958]</v>
       </c>
     </row>
     <row r="84" spans="9:15" x14ac:dyDescent="0.25">
@@ -3561,11 +3606,11 @@
       </c>
       <c r="N85" t="str">
         <f>CONCATENATE(N84,I85," - ",J85,": ",K85,IF(I86&gt;I85,"; ","]"))</f>
-        <v xml:space="preserve">[0 - 2.8: 73.02; </v>
+        <v xml:space="preserve">[0 - 2,8: 73,02; </v>
       </c>
       <c r="O85" t="str">
         <f>CONCATENATE(O84,I85, " - ",J85,": ",L85,IF(I86&gt;I85,"; ","]"))</f>
-        <v xml:space="preserve">[0 - 2.8: 0.2747; </v>
+        <v xml:space="preserve">[0 - 2,8: 0,2747; </v>
       </c>
     </row>
     <row r="86" spans="9:15" x14ac:dyDescent="0.25">
@@ -3584,11 +3629,11 @@
       </c>
       <c r="N86" t="str">
         <f t="shared" ref="N86:N89" si="8">CONCATENATE(N85,I86," - ",J86,": ",K86,IF(I87&gt;I86,"; ","]"))</f>
-        <v xml:space="preserve">[0 - 2.8: 73.02; 2.8 - 6: 92.02; </v>
+        <v xml:space="preserve">[0 - 2,8: 73,02; 2,8 - 6: 92,02; </v>
       </c>
       <c r="O86" t="str">
         <f t="shared" ref="O86:O89" si="9">CONCATENATE(O85,I86, " - ",J86,": ",L86,IF(I87&gt;I86,"; ","]"))</f>
-        <v xml:space="preserve">[0 - 2.8: 0.2747; 2.8 - 6: 0.2679; </v>
+        <v xml:space="preserve">[0 - 2,8: 0,2747; 2,8 - 6: 0,2679; </v>
       </c>
     </row>
     <row r="87" spans="9:15" x14ac:dyDescent="0.25">
@@ -3607,11 +3652,11 @@
       </c>
       <c r="N87" t="str">
         <f t="shared" si="8"/>
-        <v xml:space="preserve">[0 - 2.8: 73.02; 2.8 - 6: 92.02; 6 - 9: 99.16; </v>
+        <v xml:space="preserve">[0 - 2,8: 73,02; 2,8 - 6: 92,02; 6 - 9: 99,16; </v>
       </c>
       <c r="O87" t="str">
         <f t="shared" si="9"/>
-        <v xml:space="preserve">[0 - 2.8: 0.2747; 2.8 - 6: 0.2679; 6 - 9: 0.2667; </v>
+        <v xml:space="preserve">[0 - 2,8: 0,2747; 2,8 - 6: 0,2679; 6 - 9: 0,2667; </v>
       </c>
     </row>
     <row r="88" spans="9:15" x14ac:dyDescent="0.25">
@@ -3630,11 +3675,11 @@
       </c>
       <c r="N88" t="str">
         <f t="shared" si="8"/>
-        <v xml:space="preserve">[0 - 2.8: 73.02; 2.8 - 6: 92.02; 6 - 9: 99.16; 9 - 12: 107.73; </v>
+        <v xml:space="preserve">[0 - 2,8: 73,02; 2,8 - 6: 92,02; 6 - 9: 99,16; 9 - 12: 107,73; </v>
       </c>
       <c r="O88" t="str">
         <f t="shared" si="9"/>
-        <v xml:space="preserve">[0 - 2.8: 0.2747; 2.8 - 6: 0.2679; 6 - 9: 0.2667; 9 - 12: 0.2657; </v>
+        <v xml:space="preserve">[0 - 2,8: 0,2747; 2,8 - 6: 0,2679; 6 - 9: 0,2667; 9 - 12: 0,2657; </v>
       </c>
     </row>
     <row r="89" spans="9:15" x14ac:dyDescent="0.25">
@@ -3653,11 +3698,11 @@
       </c>
       <c r="N89" t="str">
         <f t="shared" si="8"/>
-        <v>[0 - 2.8: 73.02; 2.8 - 6: 92.02; 6 - 9: 99.16; 9 - 12: 107.73; 12 - 100: 117.73]</v>
+        <v>[0 - 2,8: 73,02; 2,8 - 6: 92,02; 6 - 9: 99,16; 9 - 12: 107,73; 12 - 100: 117,73]</v>
       </c>
       <c r="O89" t="str">
         <f t="shared" si="9"/>
-        <v>[0 - 2.8: 0.2747; 2.8 - 6: 0.2679; 6 - 9: 0.2667; 9 - 12: 0.2657; 12 - 100: 0.2649]</v>
+        <v>[0 - 2,8: 0,2747; 2,8 - 6: 0,2679; 6 - 9: 0,2667; 9 - 12: 0,2657; 12 - 100: 0,2649]</v>
       </c>
     </row>
     <row r="91" spans="9:15" x14ac:dyDescent="0.25">
@@ -3686,11 +3731,11 @@
       </c>
       <c r="N92" t="str">
         <f>CONCATENATE(N91,I92," - ",J92,": ",K92,IF(I93&gt;I92,"; ","]"))</f>
-        <v xml:space="preserve">[0 - 2.8: 73.02; </v>
+        <v xml:space="preserve">[0 - 2,8: 73,02; </v>
       </c>
       <c r="O92" t="str">
         <f>CONCATENATE(O91,I92, " - ",J92,": ",L92,IF(I93&gt;I92,"; ","]"))</f>
-        <v xml:space="preserve">[0 - 2.8: 0.2657; </v>
+        <v xml:space="preserve">[0 - 2,8: 0,2657; </v>
       </c>
     </row>
     <row r="93" spans="9:15" x14ac:dyDescent="0.25">
@@ -3709,11 +3754,11 @@
       </c>
       <c r="N93" t="str">
         <f t="shared" ref="N93:N94" si="11">CONCATENATE(N92,I93," - ",J93,": ",K93,IF(I94&gt;I93,"; ","]"))</f>
-        <v xml:space="preserve">[0 - 2.8: 73.02; 2.8 - 6: 77.02; </v>
+        <v xml:space="preserve">[0 - 2,8: 73,02; 2,8 - 6: 77,02; </v>
       </c>
       <c r="O93" t="str">
         <f t="shared" ref="O93:O94" si="12">CONCATENATE(O92,I93, " - ",J93,": ",L93,IF(I94&gt;I93,"; ","]"))</f>
-        <v xml:space="preserve">[0 - 2.8: 0.2657; 2.8 - 6: 0.2643; </v>
+        <v xml:space="preserve">[0 - 2,8: 0,2657; 2,8 - 6: 0,2643; </v>
       </c>
     </row>
     <row r="94" spans="9:15" x14ac:dyDescent="0.25">
@@ -3732,11 +3777,11 @@
       </c>
       <c r="N94" t="str">
         <f t="shared" si="11"/>
-        <v>[0 - 2.8: 73.02; 2.8 - 6: 77.02; 6 - 100: 84.16]</v>
+        <v>[0 - 2,8: 73,02; 2,8 - 6: 77,02; 6 - 100: 84,16]</v>
       </c>
       <c r="O94" t="str">
         <f t="shared" si="12"/>
-        <v>[0 - 2.8: 0.2657; 2.8 - 6: 0.2643; 6 - 100: 0.2631]</v>
+        <v>[0 - 2,8: 0,2657; 2,8 - 6: 0,2643; 6 - 100: 0,2631]</v>
       </c>
     </row>
     <row r="96" spans="9:15" x14ac:dyDescent="0.25">
@@ -3765,11 +3810,11 @@
       </c>
       <c r="N97" t="str">
         <f>CONCATENATE(N96,I97," - ",J97,": ",K97,IF(I98&gt;I97,"; ","]"))</f>
-        <v xml:space="preserve">[0 - 5.384: 39.98; </v>
+        <v xml:space="preserve">[0 - 5,384: 39,98; </v>
       </c>
       <c r="O97" t="str">
         <f>CONCATENATE(O96,I97, " - ",J97,": ",L97,IF(I98&gt;I97,"; ","]"))</f>
-        <v xml:space="preserve">[0 - 5.384: 0.0826; </v>
+        <v xml:space="preserve">[0 - 5,384: 0,0826; </v>
       </c>
     </row>
     <row r="98" spans="9:15" x14ac:dyDescent="0.25">
@@ -3788,11 +3833,11 @@
       </c>
       <c r="N98" t="str">
         <f t="shared" ref="N98:N99" si="14">CONCATENATE(N97,I98," - ",J98,": ",K98,IF(I99&gt;I98,"; ","]"))</f>
-        <v xml:space="preserve">[0 - 5.384: 39.98; 5.384 - 12.28: 138.66; </v>
+        <v xml:space="preserve">[0 - 5,384: 39,98; 5,384 - 12,28: 138,66; </v>
       </c>
       <c r="O98" t="str">
         <f t="shared" ref="O98:O99" si="15">CONCATENATE(O97,I98, " - ",J98,": ",L98,IF(I99&gt;I98,"; ","]"))</f>
-        <v xml:space="preserve">[0 - 5.384: 0.0826; 5.384 - 12.28: 0.0643; </v>
+        <v xml:space="preserve">[0 - 5,384: 0,0826; 5,384 - 12,28: 0,0643; </v>
       </c>
     </row>
     <row r="99" spans="9:15" x14ac:dyDescent="0.25">
@@ -3811,11 +3856,11 @@
       </c>
       <c r="N99" t="str">
         <f t="shared" si="14"/>
-        <v>[0 - 5.384: 39.98; 5.384 - 12.28: 138.66; 12.28 - 200: 182.5]</v>
+        <v>[0 - 5,384: 39,98; 5,384 - 12,28: 138,66; 12,28 - 200: 182,5]</v>
       </c>
       <c r="O99" t="str">
         <f t="shared" si="15"/>
-        <v>[0 - 5.384: 0.0826; 5.384 - 12.28: 0.0643; 12.28 - 200: 0.0607]</v>
+        <v>[0 - 5,384: 0,0826; 5,384 - 12,28: 0,0643; 12,28 - 200: 0,0607]</v>
       </c>
     </row>
     <row r="101" spans="9:15" x14ac:dyDescent="0.25">
@@ -3844,11 +3889,11 @@
       </c>
       <c r="N102" t="str">
         <f>CONCATENATE(N101,I102," - ",J102,": ",K102,IF(I103&gt;I102,"; ","]"))</f>
-        <v xml:space="preserve">[0 - 5.384: 39.98; </v>
+        <v xml:space="preserve">[0 - 5,384: 39,98; </v>
       </c>
       <c r="O102" t="str">
         <f>CONCATENATE(O101,I102, " - ",J102,": ",L102,IF(I103&gt;I102,"; ","]"))</f>
-        <v xml:space="preserve">[0 - 5.384: 0.0798; </v>
+        <v xml:space="preserve">[0 - 5,384: 0,0798; </v>
       </c>
     </row>
     <row r="103" spans="9:15" x14ac:dyDescent="0.25">
@@ -3867,11 +3912,11 @@
       </c>
       <c r="N103" t="str">
         <f t="shared" ref="N103:N104" si="17">CONCATENATE(N102,I103," - ",J103,": ",K103,IF(I104&gt;I103,"; ","]"))</f>
-        <v xml:space="preserve">[0 - 5.384: 39.98; 5.384 - 12.28: 138.66; </v>
+        <v xml:space="preserve">[0 - 5,384: 39,98; 5,384 - 12,28: 138,66; </v>
       </c>
       <c r="O103" t="str">
         <f t="shared" ref="O103:O104" si="18">CONCATENATE(O102,I103, " - ",J103,": ",L103,IF(I104&gt;I103,"; ","]"))</f>
-        <v xml:space="preserve">[0 - 5.384: 0.0798; 5.384 - 12.28: 0.0615; </v>
+        <v xml:space="preserve">[0 - 5,384: 0,0798; 5,384 - 12,28: 0,0615; </v>
       </c>
     </row>
     <row r="104" spans="9:15" x14ac:dyDescent="0.25">
@@ -3890,20 +3935,20 @@
       </c>
       <c r="N104" t="str">
         <f t="shared" si="17"/>
-        <v>[0 - 5.384: 39.98; 5.384 - 12.28: 138.66; 12.28 - 200: 182.5]</v>
+        <v>[0 - 5,384: 39,98; 5,384 - 12,28: 138,66; 12,28 - 200: 182,5]</v>
       </c>
       <c r="O104" t="str">
         <f t="shared" si="18"/>
-        <v>[0 - 5.384: 0.0798; 5.384 - 12.28: 0.0615; 12.28 - 200: 0.058]</v>
+        <v>[0 - 5,384: 0,0798; 5,384 - 12,28: 0,0615; 12,28 - 200: 0,058]</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D6" r:id="rId1"/>
-    <hyperlink ref="D7" r:id="rId2"/>
-    <hyperlink ref="J65" r:id="rId3"/>
-    <hyperlink ref="J52" r:id="rId4"/>
-    <hyperlink ref="J39" r:id="rId5"/>
+    <hyperlink ref="D6" r:id="rId1" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
+    <hyperlink ref="D7" r:id="rId2" xr:uid="{00000000-0004-0000-0500-000001000000}"/>
+    <hyperlink ref="J65" r:id="rId3" xr:uid="{00000000-0004-0000-0500-000002000000}"/>
+    <hyperlink ref="J52" r:id="rId4" xr:uid="{00000000-0004-0000-0500-000003000000}"/>
+    <hyperlink ref="J39" r:id="rId5" xr:uid="{00000000-0004-0000-0500-000004000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>

</xml_diff>